<commit_message>
Added larger JC variant of oscillator to the underside of the PCB
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>RJ-11</t>
   </si>
@@ -246,9 +246,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>C2, C3, C6</t>
-  </si>
-  <si>
     <t>Microcontroller</t>
   </si>
   <si>
@@ -256,6 +253,51 @@
   </si>
   <si>
     <t>40mm diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JST-EH 5 pin </t>
+  </si>
+  <si>
+    <t>socket</t>
+  </si>
+  <si>
+    <t>crimp connectors</t>
+  </si>
+  <si>
+    <t>difiKey: SER3618CT-ND</t>
+  </si>
+  <si>
+    <t>Epson/SG-3030JC 32.7680 (10.50mm x 5.00mm)</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C2, C6</t>
+  </si>
+  <si>
+    <t>Cap &gt;0.1uF (0.22uF)</t>
+  </si>
+  <si>
+    <t>digiKey: 478-8818-ND</t>
+  </si>
+  <si>
+    <t>455-1614-ND</t>
+  </si>
+  <si>
+    <t>receptacle (housing)</t>
+  </si>
+  <si>
+    <t>EHR-5</t>
+  </si>
+  <si>
+    <t>455-1003-ND</t>
+  </si>
+  <si>
+    <t>455-1042-1-ND</t>
+  </si>
+  <si>
+    <t>SEH-001T-P0.6</t>
   </si>
 </sst>
 </file>
@@ -349,7 +391,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -363,6 +405,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -658,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J27"/>
+  <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -711,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G4" si="0">E3*F3</f>
+        <f t="shared" ref="G3:G7" si="0">E3*F3</f>
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -719,491 +769,587 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>200</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="6" customFormat="1">
-      <c r="A5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="6">
-        <v>2.95</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
-        <f>E5*F5</f>
-        <v>2.95</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>7</v>
+      <c r="H5" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="E6" s="2">
-        <v>2.86</v>
+        <v>0.1</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2">
-        <f t="shared" ref="G6:G21" si="1">E6*F6</f>
-        <v>0</v>
+      <c r="H6" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>2.0299999999999998</v>
+        <v>200</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8"/>
+        <v>76</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="E8" s="6">
-        <v>0.4</v>
+        <v>2.95</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
       </c>
       <c r="G8" s="6">
+        <f>E8*F8</f>
+        <v>2.95</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.86</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" ref="G9:G25" si="1">E9*F9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="6" customFormat="1">
+      <c r="A11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="6" customFormat="1">
-      <c r="A9" s="6" t="s">
+    <row r="12" spans="1:10" s="6" customFormat="1">
+      <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
         <v>0.75</v>
       </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="1" t="s">
+    <row r="13" spans="1:10">
+      <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E13" s="2">
         <v>0.53</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F13" s="2">
         <v>2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G13" s="2">
         <f t="shared" si="1"/>
         <v>1.06</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="6" customFormat="1">
-      <c r="A11" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="6" t="s">
+    <row r="14" spans="1:10" s="6" customFormat="1">
+      <c r="A14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E14" s="6">
         <v>0.42</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.84</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="13" customFormat="1">
+      <c r="A15" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="F15" s="15">
         <v>1</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G15" s="15">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="C12" s="5" t="s">
+      <c r="H15" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G16" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="6" customFormat="1">
-      <c r="A13" s="6" t="s">
+    <row r="17" spans="1:9" s="6" customFormat="1">
+      <c r="A17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9">
         <v>0.51</v>
       </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="C14" s="2" t="s">
+    <row r="18" spans="1:9">
+      <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E18" s="2">
         <v>0.5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F18" s="2">
         <v>1</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G18" s="2">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="11" customFormat="1">
-      <c r="A15" s="11" t="s">
+    <row r="19" spans="1:9" s="11" customFormat="1">
+      <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="C19" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="11">
         <v>8</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F19" s="11">
         <v>1</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G19" s="11">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="6" customFormat="1">
-      <c r="A16" s="6" t="s">
+      <c r="H19" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1">
+      <c r="A20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E20" s="6">
         <v>3.44</v>
       </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I20" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="C17" s="1" t="s">
+    <row r="21" spans="1:9">
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.25" customHeight="1">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
+    <row r="22" spans="1:9" ht="14.25" customHeight="1">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E22" s="2">
         <v>5.23</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="G18" s="2">
-        <f>F18*E18</f>
+      <c r="G22" s="2">
+        <f>F22*E22</f>
         <v>5.23</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1">
-      <c r="A19" s="6" t="s">
+    <row r="23" spans="1:9" s="6" customFormat="1">
+      <c r="A23" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E23" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="F19" s="6">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6">
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I23" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="D20" s="2" t="s">
+    <row r="24" spans="1:9">
+      <c r="D24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E24" s="2">
         <v>2.88</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F24" s="2">
         <v>2</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G24" s="2">
         <f t="shared" si="1"/>
         <v>5.76</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="6" customFormat="1">
-      <c r="A21" s="6" t="s">
+    <row r="25" spans="1:9" s="6" customFormat="1">
+      <c r="A25" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E25" s="6">
         <v>1.58</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F25" s="6">
         <v>1</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G25" s="6">
         <f t="shared" si="1"/>
         <v>1.58</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="C22" s="1"/>
-      <c r="D22" s="12" t="s">
+    <row r="26" spans="1:9" s="13" customFormat="1">
+      <c r="C26" s="14"/>
+      <c r="D26" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1.53</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="C27" s="1"/>
+      <c r="D27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E27" s="5">
         <v>1.75</v>
       </c>
-      <c r="F22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1">
-      <c r="A23" s="6" t="s">
+    <row r="28" spans="1:9" s="6" customFormat="1">
+      <c r="A28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E28" s="6">
         <v>0.1</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F28" s="6">
         <v>1</v>
       </c>
-      <c r="G23" s="6">
-        <f>F23*E23</f>
+      <c r="G28" s="6">
+        <f>F28*E28</f>
         <v>0.1</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="6" customFormat="1">
-      <c r="A24" s="6" t="s">
+    <row r="29" spans="1:9" s="6" customFormat="1">
+      <c r="A29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F29" s="6">
         <v>3</v>
       </c>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" s="6" customFormat="1">
-      <c r="A25" s="6" t="s">
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:9" s="6" customFormat="1">
+      <c r="A30" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F30" s="6">
         <v>3</v>
       </c>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="B26" s="2" t="s">
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="F27" s="2" t="s">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="6:8">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="6:8">
+      <c r="F34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="2">
-        <f>SUM(G3:G23)</f>
-        <v>26</v>
+      <c r="G34" s="2">
+        <f>SUM(G3:G28)</f>
+        <v>26.839999999999996</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D19" r:id="rId1" display="http://www.digikey.com/en/supplier-centers/e/e-switch"/>
-    <hyperlink ref="C19" r:id="rId2"/>
-    <hyperlink ref="C17" r:id="rId3"/>
-    <hyperlink ref="D17" r:id="rId4"/>
-    <hyperlink ref="D18" r:id="rId5"/>
-    <hyperlink ref="C21" r:id="rId6" display="32.768kHz"/>
-    <hyperlink ref="C10" r:id="rId7"/>
-    <hyperlink ref="H10" r:id="rId8"/>
-    <hyperlink ref="H23" r:id="rId9"/>
-    <hyperlink ref="H22" r:id="rId10"/>
+    <hyperlink ref="D23" r:id="rId1" display="http://www.digikey.com/en/supplier-centers/e/e-switch"/>
+    <hyperlink ref="C23" r:id="rId2"/>
+    <hyperlink ref="C21" r:id="rId3"/>
+    <hyperlink ref="D21" r:id="rId4"/>
+    <hyperlink ref="D22" r:id="rId5"/>
+    <hyperlink ref="C25" r:id="rId6" display="32.768kHz"/>
+    <hyperlink ref="C13" r:id="rId7"/>
+    <hyperlink ref="H28" r:id="rId8"/>
+    <hyperlink ref="H27" r:id="rId9"/>
+    <hyperlink ref="H26" r:id="rId10"/>
+    <hyperlink ref="H13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Disable Fail-Safe Clock Monitor
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -1549,10 +1549,10 @@
   <dimension ref="A2:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>